<commit_message>
Actualiza cronograma con avances.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unmsm\plan_2015\gestion_configuracion\proyecto\SVB\Desarrollo\SVB\documentos\gestion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -175,54 +183,67 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF4285F4"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="4"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -232,7 +253,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -248,7 +269,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -262,99 +289,97 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -544,29 +569,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="C2:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.14"/>
-    <col customWidth="1" min="2" max="2" width="7.0"/>
-    <col customWidth="1" min="3" max="3" width="56.0"/>
-    <col customWidth="1" min="4" max="4" width="28.71"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D2" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="3:17" ht="15" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
@@ -613,7 +643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" ht="37.5" customHeight="1">
+    <row r="5" spans="3:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
@@ -621,7 +651,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="5">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>17</v>
@@ -638,7 +668,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6">
+    <row r="6" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
@@ -663,7 +693,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7">
+    <row r="7" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
@@ -671,7 +701,7 @@
         <v>21</v>
       </c>
       <c r="E7" s="5">
-        <v>30.0</v>
+        <v>70</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -688,7 +718,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8">
+    <row r="8" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
@@ -696,7 +726,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="7">
-        <v>40.0</v>
+        <v>60</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -715,7 +745,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9">
+    <row r="9" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>24</v>
       </c>
@@ -734,7 +764,7 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10">
+    <row r="10" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C10" s="9" t="s">
         <v>25</v>
       </c>
@@ -755,7 +785,7 @@
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11">
+    <row r="11" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C11" s="10" t="s">
         <v>27</v>
       </c>
@@ -778,7 +808,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12">
+    <row r="12" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
@@ -801,7 +831,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13">
+    <row r="13" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C13" s="11" t="s">
         <v>29</v>
       </c>
@@ -824,7 +854,7 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14">
+    <row r="14" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C14" s="10" t="s">
         <v>30</v>
       </c>
@@ -847,7 +877,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15">
+    <row r="15" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C15" s="12" t="s">
         <v>31</v>
       </c>
@@ -870,7 +900,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16">
+    <row r="16" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C16" s="13" t="s">
         <v>32</v>
       </c>
@@ -893,7 +923,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="6"/>
     </row>
-    <row r="17">
+    <row r="17" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C17" s="14" t="s">
         <v>33</v>
       </c>
@@ -916,7 +946,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18">
+    <row r="18" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C18" s="15" t="s">
         <v>34</v>
       </c>
@@ -939,7 +969,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19">
+    <row r="19" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C19" s="8" t="s">
         <v>35</v>
       </c>
@@ -958,7 +988,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20">
+    <row r="20" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C20" s="16" t="s">
         <v>36</v>
       </c>
@@ -979,14 +1009,16 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21">
+    <row r="21" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6">
+        <v>50</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -1004,7 +1036,7 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
     </row>
-    <row r="22">
+    <row r="22" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C22" s="17" t="s">
         <v>39</v>
       </c>
@@ -1027,7 +1059,7 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23">
+    <row r="23" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C23" s="17" t="s">
         <v>40</v>
       </c>
@@ -1050,7 +1082,7 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
     </row>
-    <row r="24">
+    <row r="24" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C24" s="10" t="s">
         <v>41</v>
       </c>
@@ -1077,7 +1109,7 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25">
+    <row r="25" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C25" s="10" t="s">
         <v>42</v>
       </c>
@@ -1102,7 +1134,7 @@
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26">
+    <row r="26" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C26" s="17" t="s">
         <v>43</v>
       </c>
@@ -1127,7 +1159,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27">
+    <row r="27" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C27" s="17" t="s">
         <v>44</v>
       </c>
@@ -1152,7 +1184,7 @@
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28">
+    <row r="28" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C28" s="17" t="s">
         <v>45</v>
       </c>
@@ -1177,7 +1209,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29">
+    <row r="29" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="17" t="s">
         <v>46</v>
       </c>
@@ -1200,7 +1232,7 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="6"/>
     </row>
-    <row r="30">
+    <row r="30" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C30" s="18" t="s">
         <v>47</v>
       </c>
@@ -1219,7 +1251,7 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="6"/>
     </row>
-    <row r="31">
+    <row r="31" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C31" s="19" t="s">
         <v>48</v>
       </c>
@@ -1244,7 +1276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C32" s="20" t="s">
         <v>50</v>
       </c>
@@ -1269,7 +1301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C33" s="8" t="s">
         <v>52</v>
       </c>
@@ -1289,6 +1321,6 @@
       <c r="Q33" s="24"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mejora visual de las actividades
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unmsm\plan_2015\gestion_configuracion\proyecto\SVB\Desarrollo\SVB\documentos\gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Repo\SVB\Desarrollo\SVB\documentos\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F43C726-405B-4A98-9EEB-95834E73A92E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>ACTIVIDADES</t>
   </si>
@@ -70,9 +71,6 @@
   </si>
   <si>
     <t>Gestor de documentos / Jefe de Proyecto</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>Obtención de requerimientos</t>
@@ -183,7 +181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -248,7 +246,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +263,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -295,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -357,10 +367,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,14 +594,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="C2:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -653,9 +672,7 @@
       <c r="E5" s="5">
         <v>70</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="F5" s="24"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -670,19 +687,15 @@
     </row>
     <row r="6" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -695,10 +708,10 @@
     </row>
     <row r="7" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E7" s="5">
         <v>70</v>
@@ -706,9 +719,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="I7" s="24"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -720,10 +731,10 @@
     </row>
     <row r="8" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E8" s="7">
         <v>60</v>
@@ -731,12 +742,8 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -747,7 +754,7 @@
     </row>
     <row r="9" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -766,10 +773,10 @@
     </row>
     <row r="10" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -787,20 +794,18 @@
     </row>
     <row r="11" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C11" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="6"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="27"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="5"/>
@@ -810,10 +815,10 @@
     </row>
     <row r="12" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C12" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -821,9 +826,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="K12" s="25"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="5"/>
@@ -833,10 +836,10 @@
     </row>
     <row r="13" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C13" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -844,9 +847,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="K13" s="25"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="5"/>
@@ -856,10 +857,10 @@
     </row>
     <row r="14" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C14" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -868,9 +869,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="L14" s="25"/>
       <c r="M14" s="6"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
@@ -879,10 +878,10 @@
     </row>
     <row r="15" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C15" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -891,9 +890,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="L15" s="25"/>
       <c r="M15" s="6"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -902,10 +899,10 @@
     </row>
     <row r="16" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C16" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -915,9 +912,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="M16" s="25"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
@@ -925,10 +920,10 @@
     </row>
     <row r="17" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C17" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -938,9 +933,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="M17" s="25"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -948,10 +941,10 @@
     </row>
     <row r="18" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C18" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -962,16 +955,14 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="N18" s="25"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="6"/>
     </row>
     <row r="19" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C19" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -990,10 +981,10 @@
     </row>
     <row r="20" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C20" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1011,10 +1002,10 @@
     </row>
     <row r="21" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C21" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="6">
         <v>50</v>
@@ -1022,12 +1013,8 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -1038,19 +1025,17 @@
     </row>
     <row r="22" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C22" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="J22" s="25"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -1061,10 +1046,10 @@
     </row>
     <row r="23" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C23" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -1072,9 +1057,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="K23" s="25"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
@@ -1084,10 +1067,10 @@
     </row>
     <row r="24" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C24" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1096,25 +1079,19 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
-      <c r="L24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N24" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
     </row>
     <row r="25" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C25" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -1124,22 +1101,18 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N25" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
     </row>
     <row r="26" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C26" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -1149,22 +1122,18 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N26" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
     <row r="27" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C27" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -1175,21 +1144,17 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
-      <c r="N27" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O27" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
     </row>
     <row r="28" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C28" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -1200,21 +1165,17 @@
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
-      <c r="N28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O28" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
     <row r="29" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -1226,15 +1187,13 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
-      <c r="O29" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="O29" s="25"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="6"/>
     </row>
     <row r="30" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C30" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1253,10 +1212,10 @@
     </row>
     <row r="31" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C31" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -1269,19 +1228,15 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
-      <c r="P31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q31" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
     </row>
     <row r="32" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C32" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="21" t="s">
         <v>50</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>51</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
@@ -1294,16 +1249,12 @@
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
-      <c r="P32" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q32" s="23" t="s">
-        <v>17</v>
-      </c>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
     </row>
     <row r="33" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C33" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
@@ -1318,7 +1269,7 @@
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
       <c r="P33" s="22"/>
-      <c r="Q33" s="24"/>
+      <c r="Q33" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualiza porcentajes de cronograma de actividades.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Repo\SVB\Desarrollo\SVB\documentos\gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unmsm\plan_2015\gestion_configuracion\proyecto\SVB\Desarrollo\SVB\documentos\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F43C726-405B-4A98-9EEB-95834E73A92E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>ACTIVIDADES</t>
   </si>
@@ -176,12 +175,15 @@
   </si>
   <si>
     <t>Hito: Fin de puesta en producción</t>
+  </si>
+  <si>
+    <t>Desarrollo de servicios web para la gestión de productos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -594,14 +596,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C2:Q33"/>
+  <dimension ref="C2:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -670,7 +672,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="5">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="6"/>
@@ -692,7 +694,9 @@
       <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5">
+        <v>100</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
@@ -714,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="5">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -737,7 +741,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="7">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1008,7 +1012,7 @@
         <v>36</v>
       </c>
       <c r="E21" s="6">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -1046,9 +1050,9 @@
     </row>
     <row r="23" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C23" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E23" s="6"/>
@@ -1056,8 +1060,8 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
@@ -1066,8 +1070,8 @@
       <c r="Q23" s="6"/>
     </row>
     <row r="24" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C24" s="10" t="s">
-        <v>40</v>
+      <c r="C24" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>36</v>
@@ -1078,17 +1082,17 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
     </row>
     <row r="25" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C25" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>36</v>
@@ -1100,7 +1104,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
+      <c r="L25" s="25"/>
       <c r="M25" s="25"/>
       <c r="N25" s="25"/>
       <c r="O25" s="6"/>
@@ -1108,8 +1112,8 @@
       <c r="Q25" s="6"/>
     </row>
     <row r="26" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C26" s="17" t="s">
-        <v>42</v>
+      <c r="C26" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>36</v>
@@ -1130,7 +1134,7 @@
     </row>
     <row r="27" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C27" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>36</v>
@@ -1143,15 +1147,15 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="M27" s="25"/>
       <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
+      <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
     </row>
     <row r="28" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C28" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>36</v>
@@ -1172,7 +1176,7 @@
     </row>
     <row r="29" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>36</v>
@@ -1186,16 +1190,18 @@
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
+      <c r="N29" s="25"/>
       <c r="O29" s="25"/>
-      <c r="P29" s="7"/>
+      <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
     </row>
     <row r="30" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C30" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="6"/>
+      <c r="C30" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -1206,17 +1212,15 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
-      <c r="O30" s="7"/>
+      <c r="O30" s="25"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="6"/>
     </row>
     <row r="31" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C31" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="C31" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
@@ -1227,36 +1231,38 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="25"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="6"/>
     </row>
     <row r="32" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+    </row>
+    <row r="33" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C33" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="26"/>
-      <c r="Q32" s="26"/>
-    </row>
-    <row r="33" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C33" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
@@ -1268,8 +1274,27 @@
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="23"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+    </row>
+    <row r="34" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C34" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualiza porcentajes de avance backend.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -603,7 +603,7 @@
   <dimension ref="C2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1034,7 +1034,9 @@
       <c r="D22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6">
+        <v>60</v>
+      </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1055,7 +1057,9 @@
       <c r="D23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>90</v>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>

</xml_diff>

<commit_message>
se actualizó porcentaje del Front
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unmsm\plan_2015\gestion_configuracion\proyecto\SVB\Desarrollo\SVB\documentos\gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Repo\SVB\Desarrollo\SVB\documentos\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE39B7F4-9262-47BD-8196-8A460616AFEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -183,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -596,14 +597,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="C2:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -798,12 +799,14 @@
     </row>
     <row r="11" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C11" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6">
+        <v>80</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -818,13 +821,15 @@
       <c r="Q11" s="6"/>
     </row>
     <row r="12" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C12" s="10" t="s">
-        <v>27</v>
+      <c r="C12" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6">
+        <v>80</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -839,8 +844,8 @@
       <c r="Q12" s="6"/>
     </row>
     <row r="13" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C13" s="11" t="s">
-        <v>28</v>
+      <c r="C13" t="s">
+        <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
se actualizó porcentaje de avance en front
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Repo\SVB\Desarrollo\SVB\documentos\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE39B7F4-9262-47BD-8196-8A460616AFEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5319EA-2E02-4F5B-8EB1-712D15B7DB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,7 +185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -248,6 +248,13 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -308,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -381,6 +388,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -604,7 +614,7 @@
   <dimension ref="C2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -850,7 +860,7 @@
       <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1307,5 +1317,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se actualiza el porcentaje de avance del front
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Repo\SVB\Desarrollo\SVB\documentos\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5319EA-2E02-4F5B-8EB1-712D15B7DB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398EA698-33F2-47BA-A250-1DBA55F75012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -614,7 +614,7 @@
   <dimension ref="C2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Agrega las tarea de integración al cronograma.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Repo\SVB\Desarrollo\SVB\documentos\gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\unmsm\plan_2015\gestion_configuracion\proyecto\SVB\Desarrollo\SVB\documentos\gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398EA698-33F2-47BA-A250-1DBA55F75012}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>ACTIVIDADES</t>
   </si>
@@ -179,12 +178,27 @@
   </si>
   <si>
     <t>Desarrollo de servicios web para la gestión de productos</t>
+  </si>
+  <si>
+    <t>Integración Back y Front</t>
+  </si>
+  <si>
+    <t>Despliegue de proyecto backend en la nube</t>
+  </si>
+  <si>
+    <t>Despliegue de proyecto frontend en la nube</t>
+  </si>
+  <si>
+    <t>Integración de Front con el Back</t>
+  </si>
+  <si>
+    <t>Hito: Fin de Integración</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -315,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -392,6 +406,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,14 +624,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C2:Q34"/>
+  <dimension ref="C2:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1255,12 +1272,10 @@
       <c r="Q31" s="6"/>
     </row>
     <row r="32" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="C32" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
@@ -1271,49 +1286,152 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="25"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="6"/>
     </row>
     <row r="33" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="6"/>
+    </row>
+    <row r="34" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C34" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="6"/>
+    </row>
+    <row r="35" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C35" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="6"/>
+    </row>
+    <row r="36" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C36" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="37" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C37" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="25"/>
+      <c r="Q37" s="25"/>
+    </row>
+    <row r="38" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C38" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D38" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-    </row>
-    <row r="34" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C34" s="8" t="s">
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="26"/>
+    </row>
+    <row r="39" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C39" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="23"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualiza cronograma con avances del front, registo y home.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -263,7 +263,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -404,11 +403,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,8 +629,8 @@
   </sheetPr>
   <dimension ref="C2:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -832,7 +831,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="6">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -855,7 +854,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="6">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -877,7 +876,9 @@
       <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="28"/>
+      <c r="E13" s="29">
+        <v>90</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1411,7 +1412,7 @@
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
-      <c r="P38" s="29"/>
+      <c r="P38" s="28"/>
       <c r="Q38" s="26"/>
     </row>
     <row r="39" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Actualiza cronograma con tareas de back
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -629,7 +629,7 @@
   </sheetPr>
   <dimension ref="C2:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1068,7 +1068,7 @@
         <v>36</v>
       </c>
       <c r="E22" s="6">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>

</xml_diff>

<commit_message>
Implementa servicios para el carrito de compra.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -629,8 +629,8 @@
   </sheetPr>
   <dimension ref="C2:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1091,7 +1091,7 @@
         <v>36</v>
       </c>
       <c r="E23" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -1134,7 +1134,9 @@
       <c r="D25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6">
+        <v>50</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>

</xml_diff>

<commit_message>
Actualiza cronograma con avance de pruebas.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -632,8 +632,8 @@
   </sheetPr>
   <dimension ref="C2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1414,7 +1414,9 @@
       <c r="D38" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="6">
+        <v>20</v>
+      </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>

</xml_diff>

<commit_message>
Actualiza cronograma con avances de front y back.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>ACTIVIDADES</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Desarrollo de interfaz de perfil de cliente</t>
+  </si>
+  <si>
+    <t>Desarrollo de interfaz de órdenes(carrito de compra)</t>
   </si>
 </sst>
 </file>
@@ -633,10 +636,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C2:Q40"/>
+  <dimension ref="C2:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -968,31 +971,33 @@
       <c r="Q16" s="6"/>
     </row>
     <row r="17" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C17" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6">
+        <v>100</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="7"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="25"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
     <row r="18" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C18" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E18" s="6"/>
@@ -1002,16 +1007,16 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="6"/>
     </row>
     <row r="19" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C19" s="15" t="s">
-        <v>33</v>
+      <c r="C19" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>25</v>
@@ -1026,16 +1031,20 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="25"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="6">
+        <v>100</v>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -1044,18 +1053,16 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="6"/>
     </row>
     <row r="21" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="C21" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -1065,37 +1072,35 @@
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C22" s="10" t="s">
-        <v>37</v>
+      <c r="C22" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="6">
-        <v>90</v>
-      </c>
+      <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="5"/>
     </row>
     <row r="23" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C23" s="17" t="s">
-        <v>38</v>
+      <c r="C23" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>36</v>
@@ -1106,7 +1111,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -1118,9 +1123,9 @@
     </row>
     <row r="24" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C24" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E24" s="6">
@@ -1141,9 +1146,9 @@
     </row>
     <row r="25" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C25" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E25" s="6">
@@ -1153,8 +1158,8 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
@@ -1163,8 +1168,8 @@
       <c r="Q25" s="6"/>
     </row>
     <row r="26" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C26" s="10" t="s">
-        <v>56</v>
+      <c r="C26" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>36</v>
@@ -1177,43 +1182,47 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
     <row r="27" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C27" s="10" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="6">
+        <v>100</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="30"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
       <c r="N27" s="25"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
     </row>
     <row r="28" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C28" s="17" t="s">
-        <v>40</v>
+      <c r="C28" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6">
+        <v>100</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -1229,12 +1238,14 @@
     </row>
     <row r="29" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6">
+        <v>100</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -1242,20 +1253,22 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
+      <c r="M29" s="30"/>
       <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
+      <c r="O29" s="6"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
     </row>
     <row r="30" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C30" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="6">
+        <v>50</v>
+      </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
@@ -1271,7 +1284,7 @@
     </row>
     <row r="31" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C31" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>36</v>
@@ -1285,16 +1298,18 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
+      <c r="N31" s="25"/>
       <c r="O31" s="25"/>
-      <c r="P31" s="7"/>
+      <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
     </row>
     <row r="32" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="6"/>
+      <c r="C32" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
@@ -1305,13 +1320,13 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
-      <c r="O32" s="7"/>
+      <c r="O32" s="25"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="6"/>
     </row>
     <row r="33" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C33" s="16" t="s">
-        <v>51</v>
+      <c r="C33" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1329,12 +1344,10 @@
       <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C34" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="C34" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
@@ -1344,19 +1357,21 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
       <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C35" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="6"/>
+        <v>52</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="6">
+        <v>50</v>
+      </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -1372,7 +1387,7 @@
     </row>
     <row r="36" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C36" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>25</v>
@@ -1392,10 +1407,12 @@
       <c r="Q36" s="6"/>
     </row>
     <row r="37" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C37" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="6"/>
+      <c r="C37" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -1405,21 +1422,17 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="7"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="25"/>
       <c r="Q37" s="6"/>
     </row>
     <row r="38" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C38" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="6">
-        <v>20</v>
-      </c>
+      <c r="C38" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -1429,36 +1442,40 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="25"/>
-      <c r="Q38" s="25"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="6"/>
     </row>
     <row r="39" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="6">
+        <v>20</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="25"/>
+    </row>
+    <row r="40" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C40" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D40" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="28"/>
-      <c r="Q39" s="26"/>
-    </row>
-    <row r="40" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C40" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="22"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
@@ -1470,8 +1487,27 @@
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="23"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="26"/>
+    </row>
+    <row r="41" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C41" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="22"/>
+      <c r="O41" s="22"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implementa reporte de ventas por criterios.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>ACTIVIDADES</t>
   </si>
@@ -147,12 +147,6 @@
     <t>Desarrollo de integración con pasarela de pagos.</t>
   </si>
   <si>
-    <t>Desarrollo de servicios web para los datos de los reportes.</t>
-  </si>
-  <si>
-    <t>Desarrollo de servicios web para la gestión de la contabilidad.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hito: Fin de desarrollo Back </t>
   </si>
   <si>
@@ -199,6 +193,9 @@
   </si>
   <si>
     <t>Desarrollo de interfaz de órdenes(carrito de compra)</t>
+  </si>
+  <si>
+    <t>Desarrollo de servicios web para el reporte de ventas</t>
   </si>
 </sst>
 </file>
@@ -636,10 +633,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C2:Q41"/>
+  <dimension ref="C2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -926,7 +923,7 @@
     </row>
     <row r="15" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C15" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>25</v>
@@ -1016,7 +1013,7 @@
     </row>
     <row r="19" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C19" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>25</v>
@@ -1146,7 +1143,7 @@
     </row>
     <row r="25" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C25" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>36</v>
@@ -1169,7 +1166,7 @@
     </row>
     <row r="26" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C26" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>36</v>
@@ -1192,7 +1189,7 @@
     </row>
     <row r="27" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C27" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>36</v>
@@ -1267,7 +1264,7 @@
         <v>36</v>
       </c>
       <c r="E30" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -1284,12 +1281,14 @@
     </row>
     <row r="31" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C31" s="17" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6">
+        <v>100</v>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1298,18 +1297,16 @@
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="25"/>
+      <c r="N31" s="6"/>
       <c r="O31" s="25"/>
-      <c r="P31" s="6"/>
+      <c r="P31" s="7"/>
       <c r="Q31" s="6"/>
     </row>
     <row r="32" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C32" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="C32" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
@@ -1320,13 +1317,13 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
-      <c r="O32" s="25"/>
+      <c r="O32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="6"/>
     </row>
     <row r="33" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C33" s="18" t="s">
-        <v>44</v>
+      <c r="C33" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1344,11 +1341,15 @@
       <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C34" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="C34" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="6">
+        <v>50</v>
+      </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -1357,21 +1358,19 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
       <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C35" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="6">
-        <v>50</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
@@ -1387,7 +1386,7 @@
     </row>
     <row r="36" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C36" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>25</v>
@@ -1407,12 +1406,10 @@
       <c r="Q36" s="6"/>
     </row>
     <row r="37" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C37" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="C37" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -1422,17 +1419,21 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="25"/>
-      <c r="P37" s="25"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
       <c r="Q37" s="6"/>
     </row>
     <row r="38" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C38" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="C38" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="6">
+        <v>20</v>
+      </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -1442,40 +1443,36 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="25"/>
+      <c r="Q38" s="25"/>
     </row>
     <row r="39" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="6">
-        <v>20</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="25"/>
-      <c r="Q39" s="25"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="26"/>
     </row>
     <row r="40" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="21" t="s">
-        <v>48</v>
-      </c>
+      <c r="D40" s="22"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
@@ -1487,27 +1484,8 @@
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="26"/>
-    </row>
-    <row r="41" spans="3:17" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C41" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="22"/>
-      <c r="Q41" s="23"/>
+      <c r="P40" s="22"/>
+      <c r="Q40" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualiza cronograma con avances de integración.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -635,8 +635,8 @@
   </sheetPr>
   <dimension ref="C2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1373,7 +1373,7 @@
         <v>25</v>
       </c>
       <c r="E35" s="6">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -1396,7 +1396,7 @@
         <v>25</v>
       </c>
       <c r="E36" s="6">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>

</xml_diff>

<commit_message>
Actualiza Línea base y cronograma.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
+++ b/Desarrollo/SVB/documentos/gestion/SVB-CRONOGRAMA.xlsx
@@ -635,8 +635,8 @@
   </sheetPr>
   <dimension ref="C2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -705,7 +705,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="5">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="6"/>
@@ -997,7 +997,9 @@
       <c r="D18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6">
+        <v>100</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1373,7 +1375,7 @@
         <v>25</v>
       </c>
       <c r="E35" s="6">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -1396,7 +1398,7 @@
         <v>25</v>
       </c>
       <c r="E36" s="6">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -1438,7 +1440,7 @@
         <v>44</v>
       </c>
       <c r="E38" s="6">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>

</xml_diff>